<commit_message>
aggiornato template import sportelli
</commit_message>
<xml_diff>
--- a/template/Template Sportelli Import 1.0.xlsx
+++ b/template/Template Sportelli Import 1.0.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t># Template per Import Sportelli</t>
   </si>
@@ -100,13 +100,19 @@
     <t>Lab 109</t>
   </si>
   <si>
-    <t>allenamento olimpiadi di Matematica</t>
+    <t>olimpiadi di Informatica</t>
   </si>
   <si>
-    <t>lezioni per ECDL</t>
+    <t>olimpiadi di Matematica</t>
   </si>
   <si>
-    <t>lezioni per certificazioni linguistiche</t>
+    <t>ECDL</t>
+  </si>
+  <si>
+    <t>certificazioni linguistiche ING</t>
+  </si>
+  <si>
+    <t>certificazioni linguistiche TED</t>
   </si>
 </sst>
 </file>
@@ -6880,23 +6886,28 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="10" t="s">
+      <c r="A2" s="18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="10" t="s">
+    <row r="3">
+      <c r="A3" s="18" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="5">
-      <c r="A5" s="10" t="s">
-        <v>29</v>
+      <c r="A5" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="18" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>